<commit_message>
parameter and contract address links
</commit_message>
<xml_diff>
--- a/padefi.xlsx
+++ b/padefi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>padefi smat contract :</t>
   </si>
@@ -41,9 +41,6 @@
     <t xml:space="preserve">https://testnet.bscscan.com/address/0xaf15d1f3df92da53f04590e19f09b760bab05ca7#code </t>
   </si>
   <si>
-    <t xml:space="preserve">https://testnet.bscscan.com/address/0xec34e67ed97c71f7df26b9c8ac6c075a11378632#code </t>
-  </si>
-  <si>
     <t xml:space="preserve">presale factory contract </t>
   </si>
   <si>
@@ -69,6 +66,57 @@
   </si>
   <si>
     <t>PresaleFactoryVesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0xa66b48c037a2488dd8842cb82b0d85ab9e557282#code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0xb5e508c9e2e4468d58b22735912f7f5a2d30a932#code </t>
+  </si>
+  <si>
+    <t>PadeFiVesting</t>
+  </si>
+  <si>
+    <t>https://testnet.bscscan.com/address/0x6893d69f765bd29d14c9183a29213017e31bb53b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0xa2fac5f746b4beaeaee0111c1484be2ae8cb2fb1#writeContract </t>
+  </si>
+  <si>
+    <t>presale_factory_updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0x48dfb82602106766dae688c98424fa7620d901ef#code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0xd88ca2fb546b45066ec64e0c09c7b04f9bb84786#readContract </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0x253158786c66fb6e1f510f45e5176ccbec942b5f#code </t>
+  </si>
+  <si>
+    <t>PresaleNew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0x1b7c9704454a0742c05ea111baf765c5f3d8bd4a#code </t>
+  </si>
+  <si>
+    <t>PadeFiVestingFactory</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0xbfae437a5aa57d41c677672e7f436dc944e88dcf#code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0x5e7e01d156870b3210b3712796f49ccc5c531362#code </t>
+  </si>
+  <si>
+    <t>owner set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://testnet.bscscan.com/address/0x7c47177fc170ec4cfab0d7789e7fb167340b7e71#readContract </t>
   </si>
 </sst>
 </file>
@@ -405,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,60 +488,159 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" location="readProxyContract "/>
     <hyperlink ref="A3" r:id="rId2" location="code "/>
-    <hyperlink ref="A4" r:id="rId3" location="code "/>
+    <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
     <hyperlink ref="A10" r:id="rId6" location="writeContract  "/>
     <hyperlink ref="A11" r:id="rId7" location="code "/>
+    <hyperlink ref="A14" r:id="rId8" location="code "/>
+    <hyperlink ref="A15" r:id="rId9" location="code "/>
+    <hyperlink ref="A18" r:id="rId10" location="writeContract "/>
+    <hyperlink ref="A19" r:id="rId11" location="code "/>
+    <hyperlink ref="A20" r:id="rId12" location="readContract "/>
+    <hyperlink ref="A21" r:id="rId13" location="code "/>
+    <hyperlink ref="A26" r:id="rId14" location="code "/>
+    <hyperlink ref="A27" r:id="rId15" location="code "/>
+    <hyperlink ref="A32" r:id="rId16" location="code "/>
+    <hyperlink ref="A33" r:id="rId17" location="readContract "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>